<commit_message>
Added initial UCT mapping and UML class diagram
</commit_message>
<xml_diff>
--- a/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
+++ b/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformChargeTable_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0EFB72-61B8-4CA5-9172-326FF4972C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFE223-394D-471D-B4FB-786F306D2305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$U$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -107,22 +107,22 @@
     <definedName name="Namespace_Target_RelativePath">Namespace!$M$1</definedName>
     <definedName name="Namespace_Target_Style">Namespace!$H$1</definedName>
     <definedName name="Namespace_Target_URI">Namespace!$I$1</definedName>
-    <definedName name="Property_Mapping_Code">Property!$E$1</definedName>
-    <definedName name="Property_Mapping_Description">Property!$F$1</definedName>
-    <definedName name="Property_Mapping_Notes">Property!$G$1</definedName>
+    <definedName name="Property_Mapping_Code">Property!$F$1</definedName>
+    <definedName name="Property_Mapping_Description">Property!$G$1</definedName>
+    <definedName name="Property_Mapping_Notes">Property!$H$1</definedName>
     <definedName name="Property_Source_DataType">Property!$C$1</definedName>
     <definedName name="Property_Source_Definition">Property!$D$1</definedName>
     <definedName name="Property_Source_Name">Property!$B$1</definedName>
     <definedName name="Property_Source_NamespacePrefix">Property!$A$1</definedName>
-    <definedName name="Property_Target_DataType">Property!$Q$1</definedName>
-    <definedName name="Property_Target_Definition">Property!$R$1</definedName>
-    <definedName name="Property_Target_ExampleContent">Property!$W$1</definedName>
-    <definedName name="Property_Target_Keywords">Property!$V$1</definedName>
-    <definedName name="Property_Target_Name">Property!$P$1</definedName>
-    <definedName name="Property_Target_NamespacePrefix">Property!$M$1</definedName>
-    <definedName name="Property_Target_Style">Property!$U$1</definedName>
-    <definedName name="Property_Target_SubstitutionGroup">Property!$T$1</definedName>
-    <definedName name="Property_Target_UsageInfo">Property!$X$1</definedName>
+    <definedName name="Property_Target_DataType">Property!$R$1</definedName>
+    <definedName name="Property_Target_Definition">Property!$S$1</definedName>
+    <definedName name="Property_Target_ExampleContent">Property!$X$1</definedName>
+    <definedName name="Property_Target_Keywords">Property!$W$1</definedName>
+    <definedName name="Property_Target_Name">Property!$Q$1</definedName>
+    <definedName name="Property_Target_NamespacePrefix">Property!$N$1</definedName>
+    <definedName name="Property_Target_Style">Property!$V$1</definedName>
+    <definedName name="Property_Target_SubstitutionGroup">Property!$U$1</definedName>
+    <definedName name="Property_Target_UsageInfo">Property!$Y$1</definedName>
     <definedName name="Type_Mapping_Code">Type!$E$1</definedName>
     <definedName name="Type_Mapping_Description">Type!$F$1</definedName>
     <definedName name="Type_Mapping_Notes">Type!$G$1</definedName>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="505">
   <si>
     <t>Definition</t>
   </si>
@@ -1919,9 +1919,6 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>Person Name</t>
-  </si>
-  <si>
     <t>EDM Class</t>
   </si>
   <si>
@@ -1943,15 +1940,9 @@
     <t>CodeList</t>
   </si>
   <si>
-    <t>j:ConvictionCourt?</t>
-  </si>
-  <si>
     <t>NIEM XPath</t>
   </si>
   <si>
-    <t>NIEM Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">NIEM Property Name </t>
   </si>
   <si>
@@ -2070,6 +2061,303 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>Cardinality</t>
+  </si>
+  <si>
+    <t>Nillable</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>ChargeSource</t>
+  </si>
+  <si>
+    <t>A source from which the charge was taken.</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>NIEM Type2</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nc:SourceText</t>
+  </si>
+  <si>
+    <t>nc:SourceText</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeAugmentationType</t>
+  </si>
+  <si>
+    <t>nc:TextType</t>
+  </si>
+  <si>
+    <t>A name, identifier, or reference of a resource from which the information was taken.</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>nc:Date</t>
+  </si>
+  <si>
+    <t>niem-xs:date</t>
+  </si>
+  <si>
+    <t>niem-xs:string</t>
+  </si>
+  <si>
+    <t>Statute</t>
+  </si>
+  <si>
+    <t>StatuteEffectiveDate</t>
+  </si>
+  <si>
+    <t>A date a statute/charge became effective.</t>
+  </si>
+  <si>
+    <t>nc:DateType (j:StatuteEnactmentDate)</t>
+  </si>
+  <si>
+    <t>A date a statute was enacted and came into effect.</t>
+  </si>
+  <si>
+    <t>StatuteInactiveDate</t>
+  </si>
+  <si>
+    <t>A date a statute/charge became inactive.</t>
+  </si>
+  <si>
+    <t>nc:DateType (j:StatuteRepealDate)</t>
+  </si>
+  <si>
+    <t>A date a statute was repealed and no longer applied.</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteEnactmentDate/nc:Date</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteRepealDate/nc:Date</t>
+  </si>
+  <si>
+    <t>An identification of a section or category within a code book.</t>
+  </si>
+  <si>
+    <t>nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:IdentificationIDType (j:StatuteCodeSectionIdentification)</t>
+  </si>
+  <si>
+    <t>An identification of a criminal offense within a code book.</t>
+  </si>
+  <si>
+    <t>A unique identifier of a law, rule, or ordinance within a jurisdiction that a person is accused of violating.</t>
+  </si>
+  <si>
+    <t>ChargeStatute</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteCategoryText</t>
+  </si>
+  <si>
+    <t>j:StatuteType</t>
+  </si>
+  <si>
+    <t>j:StatuteCategoryText (j:StatuteCategoryAbstract)</t>
+  </si>
+  <si>
+    <t>A kind of statute.</t>
+  </si>
+  <si>
+    <t>j:StatuteCodeIdentification?</t>
+  </si>
+  <si>
+    <t>nc:IdentificationIDType (nola-ext:StatuteCodeSectionSubparagraphIdentification)</t>
+  </si>
+  <si>
+    <t>A subparagraph description of a criminal offense within a state code book.</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/nola-ext:ChargeStatuteAugmentation/nola-ext:StatuteCodeSectionSubparagraphIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>A UCT Charge Key (Uniform Charge Table) is a shared key or identifier from a shared table that standardizes charge code definitions across the enterprise.</t>
+  </si>
+  <si>
+    <t>/j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>A plain language description of a charge.</t>
+  </si>
+  <si>
+    <t>j:ChargeType</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>ChargeStatuteDescription</t>
+  </si>
+  <si>
+    <t>A description of a statute.</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>ChargeType</t>
+  </si>
+  <si>
+    <t>A description of a crime category or the severity level to which a charge belongs.</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeSeverityText</t>
+  </si>
+  <si>
+    <t>j:ChargeSeverityText</t>
+  </si>
+  <si>
+    <t>A level of severity of a charge.</t>
+  </si>
+  <si>
+    <t>FullStatuteText</t>
+  </si>
+  <si>
+    <t>A full text of a statute or law.</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteText</t>
+  </si>
+  <si>
+    <t>j:StatuteText</t>
+  </si>
+  <si>
+    <t>The text of the offense identified in the State statute or section of a statute. A degree of involvement a person is being charged with committing in an offense.</t>
+  </si>
+  <si>
+    <t>ChargeInchoate</t>
+  </si>
+  <si>
+    <t>0..2</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>A degree of involvement a person is being charged with committing in an offense.</t>
+  </si>
+  <si>
+    <t>StatuteStatus</t>
+  </si>
+  <si>
+    <t>j:StatuteStatus</t>
+  </si>
+  <si>
+    <t>nc:StatusType</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteStatus</t>
+  </si>
+  <si>
+    <t>A current status of a statute.</t>
+  </si>
+  <si>
+    <t>EnteredOn</t>
+  </si>
+  <si>
+    <t>A data concept for a representation of a full date.</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeDocument/nc:DocumentEffectiveDate</t>
+  </si>
+  <si>
+    <t>nc:DateType</t>
+  </si>
+  <si>
+    <t>A date in which the content or action becomes enforceable, active, or effective.</t>
+  </si>
+  <si>
+    <t>EnteredBy</t>
+  </si>
+  <si>
+    <t>An entity responsible for making the resource available.This may include a person, organization or service.</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeDocument/nc:DocumentSubmitter/nc:EntityPerson/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>nc:PersonNameTextType</t>
+  </si>
+  <si>
+    <t>nc:PersonNameType (nc:DocumentSubmitter)</t>
+  </si>
+  <si>
+    <t>An entity responsible for making the resource available.</t>
+  </si>
+  <si>
+    <t>LastModifiedBy</t>
+  </si>
+  <si>
+    <t>LastModifiedDate</t>
+  </si>
+  <si>
+    <t>A date a document was last changed.</t>
+  </si>
+  <si>
+    <t>nc:DocumentType</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeDocument/nc:DocumentLastModifiedDate/nc:Date</t>
+  </si>
+  <si>
+    <t>nc:DateType (nc:DocumentEffectiveDate)</t>
+  </si>
+  <si>
+    <t>nc:Date or nc:DateTime?</t>
+  </si>
+  <si>
+    <t>A last person who contributed an entry in a document.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeDocument/nc:DocumentEntrySubmitter/nc:PersonFullName/nc:PersonName </t>
+  </si>
+  <si>
+    <t>A person who contributed an entry in a document.</t>
+  </si>
+  <si>
+    <t>nc:PersonNameType (nc:DocumentEntrySubmitter)</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>What is this flag for?</t>
   </si>
 </sst>
 </file>
@@ -2429,7 +2717,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2656,8 +2944,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -2733,7 +3024,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="124">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2741,7 +3032,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2754,120 +3045,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3560,6 +3740,126 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3831,66 +4131,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="120"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="117"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114" headerRowCellStyle="Neutral">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115" headerRowCellStyle="Neutral">
   <autoFilter ref="A31:B40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="114"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3899,8 +4199,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A2:B9" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3909,8 +4209,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A12:B17" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3919,112 +4219,113 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A20:B26" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:X21" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:X21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Definition" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="17"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="14"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="13"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="102"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="101"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y21" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Y21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="25">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
+    <tableColumn id="18" xr3:uid="{BEF724B3-88E3-4A22-BE6A-4D226C34A20A}" name="Definition" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="100"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="99"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="98"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="97"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="96"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="95"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="94"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="93"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type2" dataDxfId="92"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="90"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="89"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="86"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="85"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="84"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="94"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="92"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="91"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="90"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="89"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="88"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="87"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="86"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="85"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="70"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="69"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="74"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="73"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="72"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="71"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="70"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="69"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="68"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="67"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="66"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="53"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="52"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="51"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="50"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="49"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="52"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -6579,9 +6880,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6593,29 +6894,30 @@
     <col min="1" max="1" width="11.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.19921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.9296875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="22.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" style="2" customWidth="1"/>
-    <col min="9" max="10" width="13.06640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.06640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.06640625" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.9296875" style="83" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="19.53125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11.53125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.46484375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="4.796875" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="29.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="31.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="31.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="31.86328125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.86328125" style="2"/>
+    <col min="4" max="4" width="14.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.9296875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="22.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
+    <col min="10" max="11" width="13.06640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.06640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.06640625" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.9296875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="19.53125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.53125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.46484375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="4.796875" style="2" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="29.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="31.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="31.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="31.86328125" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -6628,551 +6930,966 @@
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="U1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="56" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="84">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="S2" s="83" t="s">
+        <v>449</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="AA2" s="83"/>
+    </row>
+    <row r="3" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E3" s="84">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" s="84">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83" t="s">
+        <v>440</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S4" s="83" t="s">
+        <v>443</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="AA4" s="82" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5" s="84">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" s="84" t="s">
+        <v>407</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="S6" s="83" t="s">
+        <v>446</v>
+      </c>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E7" s="84" t="s">
+        <v>407</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="M7" s="82" t="s">
+        <v>471</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E8" s="84" t="s">
+        <v>407</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="M8" s="82" t="s">
+        <v>471</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C9" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="84">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C10" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E10" s="84" t="s">
+        <v>408</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B11" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E11" s="84" t="s">
+        <v>408</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="84" t="s">
-        <v>367</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="56" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83" t="s">
-        <v>374</v>
-      </c>
-      <c r="C2" s="82" t="s">
+      <c r="D12" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E12" s="84">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D2" s="83" t="s">
-        <v>375</v>
-      </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
-      <c r="W2" s="83"/>
-      <c r="X2" s="83"/>
-      <c r="Z2" s="82" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.45">
-      <c r="A3" s="83"/>
-      <c r="B3" s="83" t="s">
-        <v>376</v>
-      </c>
-      <c r="C3" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D3" s="83" t="s">
-        <v>377</v>
-      </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-    </row>
-    <row r="4" spans="1:26" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="83"/>
-      <c r="B4" s="83" t="s">
-        <v>378</v>
-      </c>
-      <c r="C4" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D4" s="83" t="s">
-        <v>379</v>
-      </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="83"/>
-    </row>
-    <row r="5" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83" t="s">
-        <v>380</v>
-      </c>
-      <c r="C5" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D5" s="83" t="s">
-        <v>381</v>
-      </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="83"/>
-    </row>
-    <row r="6" spans="1:26" ht="57" x14ac:dyDescent="0.45">
-      <c r="A6" s="83"/>
-      <c r="B6" s="83" t="s">
-        <v>382</v>
-      </c>
-      <c r="C6" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D6" s="83" t="s">
-        <v>383</v>
-      </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-    </row>
-    <row r="7" spans="1:26" ht="57" x14ac:dyDescent="0.45">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83" t="s">
-        <v>384</v>
-      </c>
-      <c r="C7" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D7" s="83" t="s">
-        <v>385</v>
-      </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="83"/>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="83"/>
-    </row>
-    <row r="8" spans="1:26" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>385</v>
-      </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="83"/>
-    </row>
-    <row r="9" spans="1:26" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="83"/>
-      <c r="B9" s="83" t="s">
-        <v>387</v>
-      </c>
-      <c r="C9" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D9" s="83" t="s">
-        <v>388</v>
-      </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="83"/>
-      <c r="R9" s="83"/>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="83"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="83"/>
-    </row>
-    <row r="10" spans="1:26" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83" t="s">
-        <v>389</v>
-      </c>
-      <c r="C10" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D10" s="83" t="s">
-        <v>390</v>
-      </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="83"/>
-      <c r="T10" s="83"/>
-      <c r="U10" s="83"/>
-      <c r="V10" s="83"/>
-      <c r="W10" s="83"/>
-      <c r="X10" s="83"/>
-    </row>
-    <row r="11" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="83"/>
-      <c r="B11" s="83" t="s">
-        <v>391</v>
-      </c>
-      <c r="C11" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="D11" s="83" t="s">
+      <c r="O12" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="B13" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83"/>
-      <c r="R11" s="83"/>
-      <c r="T11" s="83"/>
-      <c r="U11" s="83"/>
-      <c r="V11" s="83"/>
-      <c r="W11" s="83"/>
-      <c r="X11" s="83"/>
-    </row>
-    <row r="12" spans="1:26" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="83"/>
-      <c r="B12" s="83" t="s">
-        <v>393</v>
-      </c>
-      <c r="C12" s="83" t="s">
-        <v>365</v>
-      </c>
-      <c r="D12" s="83" t="s">
-        <v>394</v>
-      </c>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
-      <c r="R12" s="83"/>
-      <c r="T12" s="83"/>
-      <c r="U12" s="83"/>
-      <c r="V12" s="83"/>
-      <c r="W12" s="83"/>
-      <c r="X12" s="83"/>
-    </row>
-    <row r="13" spans="1:26" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="83"/>
-      <c r="B13" s="83" t="s">
-        <v>395</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D13" s="83" t="s">
-        <v>396</v>
-      </c>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
-      <c r="R13" s="83"/>
-      <c r="T13" s="83"/>
-      <c r="U13" s="83"/>
-      <c r="V13" s="83"/>
-      <c r="W13" s="83"/>
-      <c r="X13" s="83"/>
-    </row>
-    <row r="14" spans="1:26" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="83"/>
-      <c r="B14" s="83" t="s">
-        <v>397</v>
+      <c r="D13" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E13" s="84">
+        <v>1</v>
+      </c>
+      <c r="I13" s="82" t="s">
+        <v>423</v>
+      </c>
+      <c r="J13" s="82" t="s">
+        <v>424</v>
+      </c>
+      <c r="K13" s="82" t="s">
+        <v>419</v>
+      </c>
+      <c r="L13" s="82" t="s">
+        <v>425</v>
+      </c>
+      <c r="M13" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="O13" s="82" t="s">
+        <v>432</v>
+      </c>
+      <c r="P13" s="82" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q13" s="82" t="s">
+        <v>420</v>
+      </c>
+      <c r="R13" s="82" t="s">
+        <v>421</v>
+      </c>
+      <c r="S13" s="82" t="s">
+        <v>427</v>
+      </c>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="B14" s="2" t="s">
+        <v>394</v>
       </c>
       <c r="C14" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="84">
+        <v>1</v>
+      </c>
+      <c r="I14" s="82" t="s">
+        <v>423</v>
+      </c>
+      <c r="J14" s="82" t="s">
+        <v>428</v>
+      </c>
+      <c r="K14" s="82" t="s">
+        <v>419</v>
+      </c>
+      <c r="L14" s="82" t="s">
+        <v>429</v>
+      </c>
+      <c r="M14" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="O14" s="82" t="s">
+        <v>433</v>
+      </c>
+      <c r="P14" s="82" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q14" s="82" t="s">
+        <v>420</v>
+      </c>
+      <c r="R14" s="82" t="s">
+        <v>421</v>
+      </c>
+      <c r="S14" s="82" t="s">
+        <v>431</v>
+      </c>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B15" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C15" s="82" t="s">
+        <v>364</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E15" s="84">
+        <v>1</v>
+      </c>
+      <c r="I15" s="82" t="s">
+        <v>423</v>
+      </c>
+      <c r="J15" s="82" t="s">
+        <v>475</v>
+      </c>
+      <c r="K15" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="L15" s="82" t="s">
+        <v>479</v>
+      </c>
+      <c r="M15" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82" t="s">
+        <v>478</v>
+      </c>
+      <c r="P15" s="82" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q15" s="82" t="s">
+        <v>476</v>
+      </c>
+      <c r="R15" s="82" t="s">
+        <v>477</v>
+      </c>
+      <c r="S15" s="82" t="s">
+        <v>479</v>
+      </c>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B16" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
-      <c r="R14" s="83"/>
-      <c r="T14" s="83"/>
-      <c r="U14" s="83"/>
-      <c r="V14" s="83"/>
-      <c r="W14" s="83"/>
-      <c r="X14" s="83"/>
-    </row>
-    <row r="15" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="83"/>
-      <c r="B15" s="83" t="s">
+      <c r="C16" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="82" t="s">
+        <v>486</v>
+      </c>
+      <c r="E16" s="85" t="s">
+        <v>408</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O16" s="82" t="s">
+        <v>487</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="C15" s="82" t="s">
-        <v>365</v>
-      </c>
-      <c r="D15" s="83" t="s">
-        <v>400</v>
-      </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
-      <c r="X15" s="83"/>
-    </row>
-    <row r="16" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="83"/>
-      <c r="B16" s="83" t="s">
-        <v>401</v>
-      </c>
-      <c r="C16" s="82" t="s">
-        <v>358</v>
-      </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="83"/>
-      <c r="V16" s="83"/>
-      <c r="W16" s="83"/>
-      <c r="X16" s="83"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A17" s="83"/>
-      <c r="B17" s="83" t="s">
-        <v>402</v>
       </c>
       <c r="C17" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="83"/>
-      <c r="T17" s="83"/>
-      <c r="U17" s="83"/>
-      <c r="V17" s="83"/>
-      <c r="W17" s="83"/>
-      <c r="X17" s="83"/>
-    </row>
-    <row r="18" spans="1:24" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="83"/>
-      <c r="B18" s="83" t="s">
-        <v>403</v>
+      <c r="D17" s="82" t="s">
+        <v>481</v>
+      </c>
+      <c r="E17" s="85" t="s">
+        <v>408</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O17" s="82" t="s">
+        <v>482</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="AA17" s="82" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+      <c r="B18" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>358</v>
-      </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
-      <c r="T18" s="83"/>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-      <c r="W18" s="83"/>
-      <c r="X18" s="83"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A19" s="83"/>
-      <c r="B19" s="83" t="s">
-        <v>404</v>
+        <v>412</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>499</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>408</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O18" s="82" t="s">
+        <v>500</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B19" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C19" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83"/>
-      <c r="R19" s="83"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="83"/>
-      <c r="V19" s="83"/>
-      <c r="W19" s="83"/>
-      <c r="X19" s="83"/>
-    </row>
-    <row r="20" spans="1:24" ht="114" x14ac:dyDescent="0.45">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83" t="s">
+      <c r="D19" s="82" t="s">
+        <v>494</v>
+      </c>
+      <c r="E19" s="85" t="s">
+        <v>408</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O19" s="82" t="s">
+        <v>496</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="Q19" s="83" t="s">
+        <v>420</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="AA19" s="82" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B20" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C20" s="82" t="s">
         <v>405</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="D20" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E20" s="84">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J20" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D20" s="83" t="s">
-        <v>406</v>
-      </c>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83"/>
-      <c r="R20" s="83"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="83"/>
-      <c r="V20" s="83"/>
-      <c r="W20" s="83"/>
-      <c r="X20" s="83"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83" t="s">
-        <v>407</v>
+      <c r="O20" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>357</v>
       </c>
-      <c r="D21" s="82"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
-      <c r="R21" s="83"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="83"/>
-      <c r="W21" s="83"/>
-      <c r="X21" s="83"/>
+      <c r="D21" s="82" t="s">
+        <v>503</v>
+      </c>
+      <c r="E21" s="84" t="s">
+        <v>408</v>
+      </c>
+      <c r="U21" s="2"/>
+      <c r="AA21" s="82" t="s">
+        <v>504</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="V22:V1048576 U2:U21" xr:uid="{00000000-0002-0000-0300-000002000000}">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W22:W1048576 V2:V21" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Replaced Document with AuditLog
</commit_message>
<xml_diff>
--- a/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
+++ b/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformChargeTable_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFE223-394D-471D-B4FB-786F306D2305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3352C661-058F-40C1-A6E9-2A014A6FEE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -139,7 +139,7 @@
     <definedName name="Type_Target_NamespacePrefix">Type!$H$1</definedName>
     <definedName name="Type_Target_Style">Type!$L$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="524">
   <si>
     <t>Definition</t>
   </si>
@@ -1961,21 +1961,12 @@
     <t>ChargeKey</t>
   </si>
   <si>
-    <t>a unique identifer that is to be stored as a Key in each endpoint system's statute code or charge table</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>indicates Louisiana Revises Statutes or New Orleans Municipal Code</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
-    <t>The statute Title in which a statd statute violation is found; blank for municipal ordinances</t>
-  </si>
-  <si>
     <t>ChargeViolation</t>
   </si>
   <si>
@@ -2000,21 +1991,12 @@
     <t>ChargeDescription</t>
   </si>
   <si>
-    <t>short text description of the charge. Initial values are those in current use in the Jail and Court systems on the AS400 platform</t>
-  </si>
-  <si>
     <t>LongDescription</t>
   </si>
   <si>
-    <t>possible future usage for more detailed charging language</t>
-  </si>
-  <si>
     <t>CourtType</t>
   </si>
   <si>
-    <t>indicator or the Default court to which the charge is filed (State or Municipal &amp; Traffic)</t>
-  </si>
-  <si>
     <t>ChargeClass</t>
   </si>
   <si>
@@ -2030,9 +2012,6 @@
     <t>InactiveDate</t>
   </si>
   <si>
-    <t>ending date, after which the charge is not valid</t>
-  </si>
-  <si>
     <t>InactiveReason</t>
   </si>
   <si>
@@ -2054,9 +2033,6 @@
     <t>ChargeString</t>
   </si>
   <si>
-    <t>a Concatenation of Title, ChargeViolation, ChargeSubparagraph and Class to uniquely identify a charge with a more user-readable syntax</t>
-  </si>
-  <si>
     <t>NOPDFlag</t>
   </si>
   <si>
@@ -2078,9 +2054,6 @@
     <t>ChargeSource</t>
   </si>
   <si>
-    <t>A source from which the charge was taken.</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -2354,17 +2327,101 @@
     <t>nc:PersonNameType (nc:DocumentEntrySubmitter)</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>What is this flag for?</t>
+    <t>A unique identifer that is to be stored as a Key in each endpoint system's statute code or charge table</t>
+  </si>
+  <si>
+    <t>Indicates Louisiana Revised Statutes or New Orleans Municipal Code</t>
+  </si>
+  <si>
+    <t>The statute Title in which a state statute violation is found; blank for municipal ordinances</t>
+  </si>
+  <si>
+    <t>Short text description of the charge. Initial values are those in current use in the Jail and Court systems on the AS400 platform</t>
+  </si>
+  <si>
+    <t>Detailed charging language</t>
+  </si>
+  <si>
+    <t>Indicator or the Default court to which the charge is filed (State or Municipal &amp; Traffic)</t>
+  </si>
+  <si>
+    <t>Ending date, after which the charge is not valid</t>
+  </si>
+  <si>
+    <t>Concatenation of Title, ChargeViolation, ChargeSubparagraph and Class to uniquely identify a charge with a more user-readable syntax</t>
+  </si>
+  <si>
+    <t>Boolean which NOPD will use to filter charges viewable for offense reporting in RMS</t>
+  </si>
+  <si>
+    <t>UniformChargeTableMessage</t>
+  </si>
+  <si>
+    <t>AssociationType</t>
+  </si>
+  <si>
+    <t>A formal allegation of a violation of a statute and/or ordinance in association with an arrest.</t>
+  </si>
+  <si>
+    <t>j:ChargeStatute</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute</t>
+  </si>
+  <si>
+    <t>ChargeAuditLog</t>
+  </si>
+  <si>
+    <t>AuditLog</t>
+  </si>
+  <si>
+    <t>An association of UniformChargeTable to a message.</t>
+  </si>
+  <si>
+    <t>An association of charge to an audit log,</t>
+  </si>
+  <si>
+    <t>nola-ext:UniformChargeTableMessage</t>
+  </si>
+  <si>
+    <t>nc:ObjectType</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAuditLog</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeAuditLog</t>
+  </si>
+  <si>
+    <t>nc:AssociationType</t>
+  </si>
+  <si>
+    <t>0..*</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>ChargeOffenseReportingIndicator</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeOffenseReportingIndicator</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeOffenseReportingIndicator</t>
+  </si>
+  <si>
+    <t>niem-xs:boolean</t>
+  </si>
+  <si>
+    <t>Indicates whether charges is viewable for offense reporting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2501,6 +2558,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2513,6 +2571,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2717,7 +2781,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2941,14 +3005,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -3026,33 +3096,6 @@
   </cellStyles>
   <dxfs count="124">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3867,6 +3910,33 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4143,43 +4213,43 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4227,105 +4297,105 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y21" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Y21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y24" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Y24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{BEF724B3-88E3-4A22-BE6A-4D226C34A20A}" name="Definition" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="100"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="99"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="98"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="97"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="96"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="95"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="94"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="93"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type2" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="89"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="88"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="87"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="86"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="85"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="84"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{BEF724B3-88E3-4A22-BE6A-4D226C34A20A}" name="Definition" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type2" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="70"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="69"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="68"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="51"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="49"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4626,8 +4696,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="51.265625" style="17" customWidth="1"/>
     <col min="3" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5050,10 +5120,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="3.73046875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.73046875" style="17" customWidth="1"/>
     <col min="3" max="3" width="76" style="17" customWidth="1"/>
-    <col min="4" max="5" width="29.33203125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="29.265625" style="16" customWidth="1"/>
     <col min="6" max="16384" width="8.86328125" style="16"/>
   </cols>
   <sheetData>
@@ -6734,7 +6804,7 @@
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24.1328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.46484375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="86.3984375" style="5" customWidth="1"/>
     <col min="3" max="16384" width="8.86328125" style="4"/>
   </cols>
   <sheetData>
@@ -6761,7 +6831,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="20" t="s">
         <v>50</v>
       </c>
@@ -6799,7 +6869,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>50</v>
       </c>
@@ -6827,7 +6897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="43.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
         <v>50</v>
       </c>
@@ -6880,38 +6950,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.9296875" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="22.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
-    <col min="10" max="11" width="13.06640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.06640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.06640625" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.9296875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.53125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="11.53125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.46484375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="4.796875" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="29.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="31.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="22.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="13" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.73046875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.73046875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="19.59765625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.59765625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.3984375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="4.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="29.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="17.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="31.265625" style="2" hidden="1" customWidth="1"/>
     <col min="25" max="26" width="31.86328125" style="2" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="31.86328125" style="2" customWidth="1"/>
     <col min="28" max="16384" width="8.86328125" style="2"/>
@@ -6931,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>49</v>
@@ -6964,7 +7034,7 @@
         <v>365</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>366</v>
@@ -6997,896 +7067,1021 @@
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>371</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="E2" s="84">
+        <v>494</v>
+      </c>
+      <c r="E2" s="83">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>371</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="S2" s="83" t="s">
-        <v>449</v>
+        <v>413</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>440</v>
       </c>
       <c r="U2" s="2"/>
-      <c r="AA2" s="83"/>
     </row>
     <row r="3" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" s="82" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E3" s="83">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L3" s="85" t="s">
+        <v>495</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E3" s="84">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="P3" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E4" s="84">
+        <v>496</v>
+      </c>
+      <c r="E4" s="83">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83" t="s">
-        <v>440</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="S4" s="83" t="s">
-        <v>443</v>
+      <c r="S4" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="U4" s="2"/>
       <c r="AA4" s="82" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E5" s="84">
+        <v>375</v>
+      </c>
+      <c r="E5" s="83">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E6" s="84" t="s">
-        <v>407</v>
+        <v>377</v>
+      </c>
+      <c r="E6" s="83" t="s">
+        <v>399</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="S6" s="83" t="s">
-        <v>446</v>
+        <v>413</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>437</v>
       </c>
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C7" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E7" s="84" t="s">
-        <v>407</v>
+        <v>379</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>399</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="M7" s="82" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C8" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E8" s="84" t="s">
-        <v>407</v>
+        <v>379</v>
+      </c>
+      <c r="E8" s="83" t="s">
+        <v>399</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="M8" s="82" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="U8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C9" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E9" s="84">
+        <v>497</v>
+      </c>
+      <c r="E9" s="83">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="M9" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="S9" s="2" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C10" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E10" s="84" t="s">
+        <v>498</v>
+      </c>
+      <c r="E10" s="83" t="s">
+        <v>400</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>447</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="J10" s="82" t="s">
-        <v>456</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="S10" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E11" s="84" t="s">
+        <v>499</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>400</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="S11" s="2" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>364</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E12" s="84">
+        <v>385</v>
+      </c>
+      <c r="E12" s="83">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="S12" s="2" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>220</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="E13" s="84">
+        <v>387</v>
+      </c>
+      <c r="E13" s="83">
         <v>1</v>
       </c>
       <c r="I13" s="82" t="s">
+        <v>414</v>
+      </c>
+      <c r="J13" s="82" t="s">
+        <v>415</v>
+      </c>
+      <c r="K13" s="82" t="s">
+        <v>410</v>
+      </c>
+      <c r="L13" s="82" t="s">
+        <v>416</v>
+      </c>
+      <c r="M13" s="82" t="s">
+        <v>400</v>
+      </c>
+      <c r="O13" s="82" t="s">
         <v>423</v>
       </c>
-      <c r="J13" s="82" t="s">
-        <v>424</v>
-      </c>
-      <c r="K13" s="82" t="s">
-        <v>419</v>
-      </c>
-      <c r="L13" s="82" t="s">
-        <v>425</v>
-      </c>
-      <c r="M13" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="O13" s="82" t="s">
-        <v>432</v>
-      </c>
       <c r="P13" s="82" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="Q13" s="82" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="R13" s="82" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="S13" s="82" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C14" s="82" t="s">
         <v>220</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="E14" s="84">
+        <v>500</v>
+      </c>
+      <c r="E14" s="83">
         <v>1</v>
       </c>
       <c r="I14" s="82" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J14" s="82" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="K14" s="82" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="L14" s="82" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="M14" s="82" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O14" s="82" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="P14" s="82" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="Q14" s="82" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="R14" s="82" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="S14" s="82" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C15" s="82" t="s">
         <v>364</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E15" s="84">
+        <v>390</v>
+      </c>
+      <c r="E15" s="83">
         <v>1</v>
       </c>
       <c r="I15" s="82" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="K15" s="82" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L15" s="82" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="M15" s="82" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="N15" s="82"/>
       <c r="O15" s="82" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="P15" s="82" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="Q15" s="82" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="R15" s="82" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="S15" s="82" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C16" s="82" t="s">
-        <v>412</v>
-      </c>
-      <c r="D16" s="82" t="s">
-        <v>486</v>
-      </c>
-      <c r="E16" s="85" t="s">
-        <v>408</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>94</v>
+        <v>403</v>
+      </c>
+      <c r="D16" s="82"/>
+      <c r="E16" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="I16" s="82" t="s">
+        <v>509</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O16" s="82" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C17" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="82" t="s">
-        <v>481</v>
-      </c>
-      <c r="E17" s="85" t="s">
-        <v>408</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>94</v>
+      <c r="D17" s="82"/>
+      <c r="E17" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="I17" s="82" t="s">
+        <v>509</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O17" s="82" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U17" s="2"/>
       <c r="AA17" s="82" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" spans="2:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" s="82" t="s">
+        <v>403</v>
+      </c>
+      <c r="D18" s="82"/>
+      <c r="E18" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="C18" s="82" t="s">
-        <v>412</v>
-      </c>
-      <c r="D18" s="82" t="s">
-        <v>499</v>
-      </c>
-      <c r="E18" s="85" t="s">
-        <v>408</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>94</v>
+      <c r="I18" s="82" t="s">
+        <v>509</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O18" s="82" t="s">
+        <v>491</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="S18" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="O18" s="82" t="s">
-        <v>500</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="C19" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="D19" s="82" t="s">
-        <v>494</v>
-      </c>
-      <c r="E19" s="85" t="s">
-        <v>408</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>94</v>
+      <c r="D19" s="82"/>
+      <c r="E19" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="I19" s="82" t="s">
+        <v>509</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O19" s="82" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="Q19" s="83" t="s">
-        <v>420</v>
+        <v>486</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="U19" s="2"/>
       <c r="AA19" s="82" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E20" s="83">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J20" s="82" t="s">
+        <v>447</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="E20" s="84">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="J20" s="82" t="s">
-        <v>456</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="L20" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="M20" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="S20" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C21" s="82" t="s">
         <v>357</v>
       </c>
       <c r="D21" s="82" t="s">
+        <v>502</v>
+      </c>
+      <c r="E21" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82" t="s">
+        <v>401</v>
+      </c>
+      <c r="J21" s="82" t="s">
+        <v>519</v>
+      </c>
+      <c r="K21" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="L21" s="82" t="s">
+        <v>523</v>
+      </c>
+      <c r="M21" s="82" t="s">
+        <v>400</v>
+      </c>
+      <c r="N21" s="82"/>
+      <c r="O21" s="82" t="s">
+        <v>520</v>
+      </c>
+      <c r="P21" s="82" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q21" s="82" t="s">
+        <v>521</v>
+      </c>
+      <c r="R21" s="82" t="s">
+        <v>522</v>
+      </c>
+      <c r="S21" s="82" t="s">
+        <v>523</v>
+      </c>
+      <c r="T21" s="82"/>
+      <c r="U21" s="82" t="s">
+        <v>400</v>
+      </c>
+      <c r="AA21" s="87"/>
+    </row>
+    <row r="22" spans="2:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="D22" s="82"/>
+      <c r="E22" s="84">
+        <v>1</v>
+      </c>
+      <c r="J22" s="82" t="s">
         <v>503</v>
       </c>
-      <c r="E21" s="84" t="s">
-        <v>408</v>
-      </c>
-      <c r="U21" s="2"/>
-      <c r="AA21" s="82" t="s">
+      <c r="K22" s="82" t="s">
         <v>504</v>
+      </c>
+      <c r="L22" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="M22" s="84">
+        <v>1</v>
+      </c>
+      <c r="O22" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="R22" s="82" t="s">
+        <v>513</v>
+      </c>
+      <c r="S22" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="U22" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D23" s="82"/>
+      <c r="E23" s="84" t="s">
+        <v>517</v>
+      </c>
+      <c r="J23" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="K23" s="82" t="s">
+        <v>504</v>
+      </c>
+      <c r="L23" s="82" t="s">
+        <v>511</v>
+      </c>
+      <c r="M23" s="84" t="s">
+        <v>517</v>
+      </c>
+      <c r="O23" s="82" t="s">
+        <v>514</v>
+      </c>
+      <c r="P23" s="82" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q23" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="R23" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="S23" s="82" t="s">
+        <v>511</v>
+      </c>
+      <c r="U23" s="84" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="D24" s="82"/>
+      <c r="E24" s="84">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="M24" s="86">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="U24" s="86">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations disablePrompts="1" count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W22:W1048576 V2:V21" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W22:W1048576 V2:V24" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
@@ -7917,17 +8112,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="29.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="29.73046875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.73046875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.1328125" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="29.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="45.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.53125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="45.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="29.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="45.73046875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.59765625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="45.73046875" style="2" customWidth="1"/>
     <col min="15" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
@@ -8009,22 +8204,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.1328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="29.73046875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.73046875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.73046875" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" style="2" customWidth="1"/>
     <col min="11" max="11" width="23.86328125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="14.46484375" style="17" customWidth="1"/>
-    <col min="16" max="16" width="43.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="30.73046875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" style="17" customWidth="1"/>
+    <col min="15" max="15" width="14.3984375" style="17" customWidth="1"/>
+    <col min="16" max="16" width="43.73046875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.73046875" style="2" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
@@ -8116,18 +8311,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.46484375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.73046875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.265625" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" style="17" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="16.86328125" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="12.265625" style="17" customWidth="1"/>
     <col min="10" max="10" width="32.86328125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="17.46484375" style="17" customWidth="1"/>
-    <col min="12" max="12" width="40.6640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="40.73046875" style="17" customWidth="1"/>
     <col min="13" max="13" width="22.1328125" style="17" customWidth="1"/>
     <col min="14" max="16384" width="8.86328125" style="17"/>
   </cols>
@@ -8209,19 +8404,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" style="58" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.73046875" style="58" customWidth="1"/>
+    <col min="3" max="3" width="35.73046875" style="58" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="6" width="29.1328125" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="58" customWidth="1"/>
+    <col min="7" max="7" width="23.73046875" style="58" customWidth="1"/>
     <col min="8" max="8" width="13" style="58" customWidth="1"/>
-    <col min="9" max="9" width="55.6640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" style="58" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.53125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="35.46484375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" style="59" customWidth="1"/>
+    <col min="9" max="9" width="55.73046875" style="58" customWidth="1"/>
+    <col min="10" max="10" width="35.73046875" style="58" customWidth="1"/>
+    <col min="11" max="11" width="14.73046875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.59765625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.3984375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.73046875" style="59" customWidth="1"/>
     <col min="15" max="15" width="9.1328125" style="2" customWidth="1"/>
     <col min="16" max="16384" width="8.86328125" style="2"/>
   </cols>
@@ -8307,15 +8502,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="4" width="20.53125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="17" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="20.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.265625" style="17" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="16.86328125" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.73046875" style="2" customWidth="1"/>
     <col min="10" max="10" width="23.86328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.73046875" style="2" customWidth="1"/>
     <col min="12" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
@@ -8367,4 +8562,327 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Updates xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099718ADBC551F541BC88D358FCBE0BE1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="431516bc1bae45c9da16ea2d2733f767">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xmlns:ns3="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b847ca3903a29a1cc3194747c84dee6d" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
+    <xsd:import namespace="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:Updates" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="21" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="22" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2666cf29-b4bf-4847-95b3-6cedd838a2fd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="abb12ba4-be90-464f-b02c-3d5a455f49fb" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="19" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Updates" ma:index="24" nillable="true" ma:displayName="Updates" ma:format="Dropdown" ma:internalName="Updates">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="12" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{84d0a8af-dfdc-4aca-88eb-038b6c01883c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="b2317584-b0e7-4f0b-a0b2-363e6e597dc0">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2AE94B-495A-4017-A3D0-1724D4100D07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B05EF41-DB28-4C2E-A8E7-8EFEC28FA29F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB52426-5EDD-49C9-B37C-4AE9ED6E055B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
+    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
First complete subset, extension and instance
</commit_message>
<xml_diff>
--- a/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
+++ b/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformChargeTable_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08D307-8888-4319-B594-5317AA2D5A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42556C3C-1DA8-4DB5-B377-027B48DEAB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2168,9 +2168,6 @@
     <t>A UCT Charge Key (Uniform Charge Table) is a shared key or identifier from a shared table that standardizes charge code definitions across the enterprise.</t>
   </si>
   <si>
-    <t>/j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeKey</t>
-  </si>
-  <si>
     <t>nola-ext:ChargeKey</t>
   </si>
   <si>
@@ -2246,15 +2243,6 @@
     <t>StatuteStatus</t>
   </si>
   <si>
-    <t>j:StatuteStatus</t>
-  </si>
-  <si>
-    <t>nc:StatusType</t>
-  </si>
-  <si>
-    <t>j:Charge/j:ChargeStatute/j:StatuteStatus</t>
-  </si>
-  <si>
     <t>A current status of a statute.</t>
   </si>
   <si>
@@ -2387,9 +2375,6 @@
     <t>nc:ObjectType</t>
   </si>
   <si>
-    <t>j:Charge/nola-ext:ChargeAuditLog</t>
-  </si>
-  <si>
     <t>nola-ext:ChargeAuditLog</t>
   </si>
   <si>
@@ -2421,6 +2406,21 @@
   </si>
   <si>
     <t>An indicator whether a charge is viewable for offense reporting</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteStatus/j:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>nc:StatusType (j:StatuteStatus)</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeAuditLog</t>
   </si>
 </sst>
 </file>
@@ -4299,6 +4299,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y24" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:Y24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y24">
+    <sortCondition ref="O1:O24"/>
+  </sortState>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
@@ -6953,10 +6956,10 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7075,7 +7078,7 @@
         <v>397</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E2" s="83">
         <v>1</v>
@@ -7096,13 +7099,13 @@
         <v>400</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>441</v>
+        <v>521</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>407</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>413</v>
@@ -7114,319 +7117,304 @@
     </row>
     <row r="3" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C3" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E3" s="83">
-        <v>1</v>
+        <v>379</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>399</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>401</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>402</v>
+        <v>460</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L3" s="85" t="s">
-        <v>495</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>400</v>
+      <c r="L3" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="M3" s="82" t="s">
+        <v>461</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>405</v>
+        <v>462</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>407</v>
+        <v>443</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>406</v>
+        <v>463</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>408</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>409</v>
+        <v>464</v>
       </c>
       <c r="U3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C4" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="E4" s="83">
-        <v>1</v>
+        <v>379</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>399</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>430</v>
+        <v>460</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>400</v>
+        <v>459</v>
+      </c>
+      <c r="M4" s="82" t="s">
+        <v>461</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>431</v>
+        <v>462</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>433</v>
+        <v>463</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>408</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>434</v>
+        <v>464</v>
       </c>
       <c r="U4" s="2"/>
       <c r="AA4" s="82" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="C5" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>375</v>
+        <v>493</v>
       </c>
       <c r="E5" s="83">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>426</v>
+        <v>445</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C6" s="82" t="s">
-        <v>397</v>
+        <v>384</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="E6" s="83" t="s">
-        <v>399</v>
+        <v>385</v>
+      </c>
+      <c r="E6" s="83">
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>376</v>
+        <v>450</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>426</v>
+        <v>453</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B7" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C7" s="82" t="s">
-        <v>397</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E7" s="83" t="s">
-        <v>399</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>401</v>
+    <row r="7" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="D7" s="82"/>
+      <c r="E7" s="84">
+        <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>403</v>
+        <v>500</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="M7" s="82" t="s">
-        <v>462</v>
+        <v>501</v>
+      </c>
+      <c r="M7" s="83">
+        <v>1</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>444</v>
+        <v>503</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>464</v>
+        <v>502</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+        <v>432</v>
+      </c>
+      <c r="U7" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C8" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E8" s="83" t="s">
-        <v>399</v>
+        <v>492</v>
+      </c>
+      <c r="E8" s="83">
+        <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="M8" s="82" t="s">
-        <v>462</v>
+        <v>429</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>464</v>
+        <v>433</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>408</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C9" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>497</v>
+        <v>375</v>
       </c>
       <c r="E9" s="83">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="U9" s="2"/>
     </row>
@@ -7438,7 +7426,7 @@
         <v>397</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="E10" s="83" t="s">
         <v>400</v>
@@ -7447,133 +7435,133 @@
         <v>414</v>
       </c>
       <c r="J10" s="82" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>432</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>408</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>397</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="E11" s="83" t="s">
-        <v>400</v>
+        <v>497</v>
+      </c>
+      <c r="E11" s="83">
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>456</v>
+      <c r="J11" s="82" t="s">
+        <v>446</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>432</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>408</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>364</v>
+        <v>386</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>220</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E12" s="83">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="M12" s="2" t="s">
+      <c r="I12" s="82" t="s">
+        <v>414</v>
+      </c>
+      <c r="J12" s="82" t="s">
+        <v>415</v>
+      </c>
+      <c r="K12" s="82" t="s">
+        <v>410</v>
+      </c>
+      <c r="L12" s="82" t="s">
+        <v>416</v>
+      </c>
+      <c r="M12" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>455</v>
+      <c r="O12" s="82" t="s">
+        <v>423</v>
+      </c>
+      <c r="P12" s="82" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q12" s="82" t="s">
+        <v>411</v>
+      </c>
+      <c r="R12" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="S12" s="82" t="s">
+        <v>418</v>
       </c>
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C13" s="82" t="s">
         <v>220</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>387</v>
+        <v>496</v>
       </c>
       <c r="E13" s="83">
         <v>1</v>
@@ -7582,22 +7570,22 @@
         <v>414</v>
       </c>
       <c r="J13" s="82" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="K13" s="82" t="s">
         <v>410</v>
       </c>
       <c r="L13" s="82" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="M13" s="82" t="s">
         <v>400</v>
       </c>
       <c r="O13" s="82" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="P13" s="82" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="Q13" s="82" t="s">
         <v>411</v>
@@ -7606,19 +7594,19 @@
         <v>412</v>
       </c>
       <c r="S13" s="82" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C14" s="82" t="s">
-        <v>220</v>
+        <v>364</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>500</v>
+        <v>390</v>
       </c>
       <c r="E14" s="83">
         <v>1</v>
@@ -7627,215 +7615,212 @@
         <v>414</v>
       </c>
       <c r="J14" s="82" t="s">
-        <v>419</v>
+        <v>465</v>
       </c>
       <c r="K14" s="82" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="L14" s="82" t="s">
-        <v>420</v>
+        <v>466</v>
       </c>
       <c r="M14" s="82" t="s">
         <v>400</v>
       </c>
+      <c r="N14" s="82"/>
       <c r="O14" s="82" t="s">
-        <v>424</v>
+        <v>522</v>
       </c>
       <c r="P14" s="82" t="s">
-        <v>421</v>
+        <v>524</v>
       </c>
       <c r="Q14" s="82" t="s">
-        <v>411</v>
+        <v>523</v>
       </c>
       <c r="R14" s="82" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="S14" s="82" t="s">
-        <v>422</v>
+        <v>466</v>
       </c>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C15" s="82" t="s">
-        <v>364</v>
+        <v>397</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E15" s="83">
-        <v>1</v>
-      </c>
-      <c r="I15" s="82" t="s">
+        <v>495</v>
+      </c>
+      <c r="E15" s="83" t="s">
+        <v>400</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J15" s="82" t="s">
-        <v>466</v>
-      </c>
-      <c r="K15" s="82" t="s">
+      <c r="J15" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L15" s="82" t="s">
-        <v>470</v>
-      </c>
-      <c r="M15" s="82" t="s">
+      <c r="L15" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82" t="s">
-        <v>469</v>
-      </c>
-      <c r="P15" s="82" t="s">
+      <c r="O15" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="Q15" s="82" t="s">
-        <v>467</v>
-      </c>
-      <c r="R15" s="82" t="s">
-        <v>468</v>
-      </c>
-      <c r="S15" s="82" t="s">
-        <v>470</v>
+      <c r="Q15" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>456</v>
       </c>
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="C16" s="82" t="s">
-        <v>403</v>
-      </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="84" t="s">
-        <v>400</v>
-      </c>
-      <c r="I16" s="82" t="s">
-        <v>509</v>
+        <v>397</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E16" s="83" t="s">
+        <v>399</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>414</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>476</v>
+        <v>376</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>477</v>
+        <v>437</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O16" s="82" t="s">
-        <v>478</v>
+      <c r="O16" s="2" t="s">
+        <v>439</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>479</v>
+        <v>426</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>480</v>
+        <v>413</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>482</v>
+        <v>437</v>
       </c>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C17" s="82" t="s">
-        <v>220</v>
-      </c>
+    <row r="17" spans="2:27" ht="71.25" x14ac:dyDescent="0.45">
       <c r="D17" s="82"/>
       <c r="E17" s="84" t="s">
-        <v>400</v>
-      </c>
-      <c r="I17" s="82" t="s">
-        <v>509</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>400</v>
+        <v>511</v>
+      </c>
+      <c r="J17" s="82" t="s">
+        <v>504</v>
+      </c>
+      <c r="K17" s="82" t="s">
+        <v>500</v>
+      </c>
+      <c r="L17" s="82" t="s">
+        <v>519</v>
+      </c>
+      <c r="M17" s="84" t="s">
+        <v>511</v>
       </c>
       <c r="O17" s="82" t="s">
-        <v>473</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="U17" s="2"/>
+        <v>525</v>
+      </c>
+      <c r="P17" s="82" t="s">
+        <v>443</v>
+      </c>
+      <c r="Q17" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="R17" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="S17" s="82" t="s">
+        <v>507</v>
+      </c>
+      <c r="U17" s="84" t="s">
+        <v>511</v>
+      </c>
       <c r="AA17" s="82" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>403</v>
-      </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="84" t="s">
-        <v>400</v>
-      </c>
-      <c r="I18" s="82" t="s">
-        <v>509</v>
+        <v>397</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E18" s="83">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>483</v>
+        <v>402</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>490</v>
+      <c r="L18" s="85" t="s">
+        <v>491</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O18" s="82" t="s">
-        <v>491</v>
+        <v>405</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>493</v>
+        <v>407</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>479</v>
+        <v>406</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>480</v>
+        <v>408</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>492</v>
+        <v>409</v>
       </c>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C19" s="82" t="s">
         <v>220</v>
@@ -7845,205 +7830,219 @@
         <v>400</v>
       </c>
       <c r="I19" s="82" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>410</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>400</v>
       </c>
       <c r="O19" s="82" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>411</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="U19" s="2"/>
       <c r="AA19" s="82" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>397</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E20" s="83">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="J20" s="82" t="s">
-        <v>447</v>
+        <v>403</v>
+      </c>
+      <c r="D20" s="82"/>
+      <c r="E20" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="I20" s="82" t="s">
+        <v>505</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>479</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>403</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>448</v>
+        <v>486</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>449</v>
+      <c r="O20" s="82" t="s">
+        <v>487</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>432</v>
+        <v>489</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>450</v>
+        <v>475</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>408</v>
+        <v>476</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>448</v>
+        <v>488</v>
       </c>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>357</v>
-      </c>
-      <c r="D21" s="82" t="s">
-        <v>502</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="D21" s="82"/>
       <c r="E21" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
       <c r="I21" s="82" t="s">
+        <v>505</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O21" s="82" t="s">
+        <v>483</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C22" s="82" t="s">
+        <v>403</v>
+      </c>
+      <c r="D22" s="82"/>
+      <c r="E22" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="I22" s="82" t="s">
+        <v>505</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O22" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C23" s="82" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" s="82" t="s">
+        <v>498</v>
+      </c>
+      <c r="E23" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82" t="s">
         <v>401</v>
       </c>
-      <c r="J21" s="82" t="s">
-        <v>518</v>
-      </c>
-      <c r="K21" s="82" t="s">
-        <v>517</v>
-      </c>
-      <c r="L21" s="82" t="s">
-        <v>525</v>
-      </c>
-      <c r="M21" s="82" t="s">
+      <c r="J23" s="82" t="s">
+        <v>513</v>
+      </c>
+      <c r="K23" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="L23" s="82" t="s">
+        <v>520</v>
+      </c>
+      <c r="M23" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82" t="s">
-        <v>519</v>
-      </c>
-      <c r="P21" s="82" t="s">
-        <v>407</v>
-      </c>
-      <c r="Q21" s="82" t="s">
-        <v>520</v>
-      </c>
-      <c r="R21" s="82" t="s">
-        <v>521</v>
-      </c>
-      <c r="S21" s="82" t="s">
-        <v>522</v>
-      </c>
-      <c r="T21" s="82"/>
-      <c r="U21" s="82" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="22" spans="2:27" ht="57" x14ac:dyDescent="0.45">
-      <c r="D22" s="82"/>
-      <c r="E22" s="84">
-        <v>1</v>
-      </c>
-      <c r="J22" s="82" t="s">
-        <v>503</v>
-      </c>
-      <c r="K22" s="82" t="s">
-        <v>504</v>
-      </c>
-      <c r="L22" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="M22" s="84">
-        <v>1</v>
-      </c>
-      <c r="O22" s="82" t="s">
-        <v>512</v>
-      </c>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="82" t="s">
-        <v>512</v>
-      </c>
-      <c r="R22" s="82" t="s">
-        <v>513</v>
-      </c>
-      <c r="S22" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="U22" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="D23" s="82"/>
-      <c r="E23" s="84" t="s">
-        <v>516</v>
-      </c>
-      <c r="J23" s="82" t="s">
-        <v>508</v>
-      </c>
-      <c r="K23" s="82" t="s">
-        <v>504</v>
-      </c>
-      <c r="L23" s="82" t="s">
-        <v>524</v>
-      </c>
-      <c r="M23" s="84" t="s">
-        <v>516</v>
-      </c>
+      <c r="N23" s="82"/>
       <c r="O23" s="82" t="s">
         <v>514</v>
       </c>
       <c r="P23" s="82" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
       <c r="Q23" s="82" t="s">
         <v>515</v>
       </c>
       <c r="R23" s="82" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="S23" s="82" t="s">
-        <v>511</v>
-      </c>
-      <c r="U23" s="84" t="s">
-        <v>516</v>
+        <v>517</v>
+      </c>
+      <c r="T23" s="82"/>
+      <c r="U23" s="82" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="2:27" ht="57" x14ac:dyDescent="0.45">
@@ -8051,28 +8050,32 @@
       <c r="E24" s="84">
         <v>1</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="M24" s="83">
+      <c r="J24" s="82" t="s">
+        <v>499</v>
+      </c>
+      <c r="K24" s="82" t="s">
+        <v>500</v>
+      </c>
+      <c r="L24" s="82" t="s">
+        <v>506</v>
+      </c>
+      <c r="M24" s="84">
         <v>1</v>
       </c>
-      <c r="O24" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="Q24" s="2" t="s">
+      <c r="O24" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="R24" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="S24" s="82" t="s">
         <v>506</v>
       </c>
-      <c r="R24" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="U24" s="83">
+      <c r="U24" s="84">
         <v>1</v>
       </c>
     </row>
@@ -8564,6 +8567,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Updates xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099718ADBC551F541BC88D358FCBE0BE1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="431516bc1bae45c9da16ea2d2733f767">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xmlns:ns3="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b847ca3903a29a1cc3194747c84dee6d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8817,45 +8843,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Updates xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB52426-5EDD-49C9-B37C-4AE9ED6E055B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2AE94B-495A-4017-A3D0-1724D4100D07}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
-    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8879,9 +8870,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2AE94B-495A-4017-A3D0-1724D4100D07}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB52426-5EDD-49C9-B37C-4AE9ED6E055B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
+    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Long Description and comments to example
</commit_message>
<xml_diff>
--- a/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
+++ b/schemas/UniformChargeTable_iepd/artifacts/UniformChargeTable_MappingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformChargeTable_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42556C3C-1DA8-4DB5-B377-027B48DEAB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1A3172-46D4-4DE7-8C46-B5FC14692ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$W$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -107,22 +107,22 @@
     <definedName name="Namespace_Target_RelativePath">Namespace!$M$1</definedName>
     <definedName name="Namespace_Target_Style">Namespace!$H$1</definedName>
     <definedName name="Namespace_Target_URI">Namespace!$I$1</definedName>
-    <definedName name="Property_Mapping_Code">Property!$F$1</definedName>
-    <definedName name="Property_Mapping_Description">Property!$G$1</definedName>
-    <definedName name="Property_Mapping_Notes">Property!$H$1</definedName>
+    <definedName name="Property_Mapping_Code">Property!$G$1</definedName>
+    <definedName name="Property_Mapping_Description">Property!$H$1</definedName>
+    <definedName name="Property_Mapping_Notes">Property!$I$1</definedName>
     <definedName name="Property_Source_DataType">Property!$C$1</definedName>
     <definedName name="Property_Source_Definition">Property!$D$1</definedName>
     <definedName name="Property_Source_Name">Property!$B$1</definedName>
     <definedName name="Property_Source_NamespacePrefix">Property!$A$1</definedName>
-    <definedName name="Property_Target_DataType">Property!$R$1</definedName>
-    <definedName name="Property_Target_Definition">Property!$S$1</definedName>
-    <definedName name="Property_Target_ExampleContent">Property!$X$1</definedName>
-    <definedName name="Property_Target_Keywords">Property!$W$1</definedName>
-    <definedName name="Property_Target_Name">Property!$Q$1</definedName>
-    <definedName name="Property_Target_NamespacePrefix">Property!$N$1</definedName>
-    <definedName name="Property_Target_Style">Property!$V$1</definedName>
-    <definedName name="Property_Target_SubstitutionGroup">Property!$U$1</definedName>
-    <definedName name="Property_Target_UsageInfo">Property!$Y$1</definedName>
+    <definedName name="Property_Target_DataType">Property!$S$1</definedName>
+    <definedName name="Property_Target_Definition">Property!$T$1</definedName>
+    <definedName name="Property_Target_ExampleContent">Property!$Y$1</definedName>
+    <definedName name="Property_Target_Keywords">Property!$X$1</definedName>
+    <definedName name="Property_Target_Name">Property!$R$1</definedName>
+    <definedName name="Property_Target_NamespacePrefix">Property!$O$1</definedName>
+    <definedName name="Property_Target_Style">Property!$W$1</definedName>
+    <definedName name="Property_Target_SubstitutionGroup">Property!$V$1</definedName>
+    <definedName name="Property_Target_UsageInfo">Property!$Z$1</definedName>
     <definedName name="Type_Mapping_Code">Type!$E$1</definedName>
     <definedName name="Type_Mapping_Description">Type!$F$1</definedName>
     <definedName name="Type_Mapping_Notes">Type!$G$1</definedName>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="539">
   <si>
     <t>Definition</t>
   </si>
@@ -2138,21 +2138,9 @@
     <t>ChargeStatute</t>
   </si>
   <si>
-    <t>j:Charge/j:ChargeStatute/j:StatuteCategoryText</t>
-  </si>
-  <si>
     <t>j:StatuteType</t>
   </si>
   <si>
-    <t>j:StatuteCategoryText (j:StatuteCategoryAbstract)</t>
-  </si>
-  <si>
-    <t>A kind of statute.</t>
-  </si>
-  <si>
-    <t>j:StatuteCodeIdentification?</t>
-  </si>
-  <si>
     <t>nc:IdentificationIDType (nola-ext:StatuteCodeSectionSubparagraphIdentification)</t>
   </si>
   <si>
@@ -2421,6 +2409,57 @@
   </si>
   <si>
     <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeAuditLog</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>ChargeCategoryType</t>
+  </si>
+  <si>
+    <t>A description of a crime category.</t>
+  </si>
+  <si>
+    <t>j:ChargeCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>j:Charge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType (j:StatuteCodeIdentification)</t>
+  </si>
+  <si>
+    <t>An identification number of a set of laws for a particular jurisdiction.</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>ATT THEFT $1499 TO $4999</t>
+  </si>
+  <si>
+    <t>(27)67(B)(2)</t>
+  </si>
+  <si>
+    <t>14:(27)67(B)(2)23D</t>
+  </si>
+  <si>
+    <t>Repeal</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>23D</t>
+  </si>
+  <si>
+    <t>LA R.S.</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>John Doe</t>
   </si>
 </sst>
 </file>
@@ -2787,7 +2826,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3020,6 +3059,18 @@
     <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -3094,7 +3145,16 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="125">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4201,66 +4261,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:D13" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Document" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source fields_x000a_(blue column headers)" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Target fields_x000a_(red column headers)" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115" headerRowCellStyle="Neutral">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A31:B40" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117" tableBorderDxfId="116" headerRowCellStyle="Neutral">
   <autoFilter ref="A31:B40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tips and tricks" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4269,8 +4329,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A2:B9" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SOURCE INFORMATION" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" " dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4279,8 +4339,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A12:B17" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="109"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="MAPPING INFORMATION" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name=" " dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4289,116 +4349,117 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A20:B26" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TARGET INFORMATION" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name=" " dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y24" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Y24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y24">
-    <sortCondition ref="O1:O24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Z24" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Z24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z24">
+    <sortCondition ref="P1:P24"/>
   </sortState>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{BEF724B3-88E3-4A22-BE6A-4D226C34A20A}" name="Definition" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cardinality" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type2" dataDxfId="89"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="103"/>
+    <tableColumn id="18" xr3:uid="{BEF724B3-88E3-4A22-BE6A-4D226C34A20A}" name="Definition" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{FE699FA9-A675-4258-A4B1-651316A0B37D}" name="Cardinality" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Example" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="98"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="97"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="96"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="95"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="94"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="93"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="92"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="91"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type2" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="88"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="87"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="84"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="83"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="82"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="70"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="68"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="66"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="49"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="47"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -6953,13 +7014,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AB24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6967,30 +7028,30 @@
     <col min="1" max="1" width="11.73046875" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="22.73046875" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" style="2" customWidth="1"/>
-    <col min="10" max="11" width="13" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.73046875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="16" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.73046875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.59765625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="11.59765625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.3984375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="4.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="29.73046875" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="17.265625" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="31.265625" style="2" hidden="1" customWidth="1"/>
-    <col min="25" max="26" width="31.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="31.86328125" style="2" customWidth="1"/>
-    <col min="28" max="16384" width="8.86328125" style="2"/>
+    <col min="4" max="5" width="14.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="22.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.86328125" style="2" customWidth="1"/>
+    <col min="11" max="12" width="13" style="2" customWidth="1"/>
+    <col min="13" max="13" width="22.73046875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.73046875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.59765625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="11.59765625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.3984375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="29.73046875" style="2" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="17.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="31.265625" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="31.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="31.86328125" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="8.86328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" s="56" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -7006,71 +7067,74 @@
       <c r="E1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="56" t="s">
+      <c r="AB1" s="56" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>371</v>
       </c>
@@ -7078,44 +7142,47 @@
         <v>397</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E2" s="83">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="F2" s="83">
+        <v>1125</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>440</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>521</v>
-      </c>
       <c r="P2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>441</v>
-      </c>
       <c r="R2" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="T2" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>378</v>
       </c>
@@ -7128,39 +7195,42 @@
       <c r="E3" s="83" t="s">
         <v>399</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="F3" s="87">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="N3" s="82" t="s">
+        <v>457</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="M3" s="82" t="s">
-        <v>461</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>380</v>
       </c>
@@ -7173,42 +7243,41 @@
       <c r="E4" s="83" t="s">
         <v>399</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="F4" s="83"/>
+      <c r="J4" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="N4" s="82" t="s">
+        <v>457</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="M4" s="82" t="s">
-        <v>461</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="AA4" s="82" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="V4" s="2"/>
+      <c r="AB4" s="86"/>
+    </row>
+    <row r="5" spans="1:28" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>381</v>
       </c>
@@ -7216,44 +7285,47 @@
         <v>397</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E5" s="83">
         <v>1</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="F5" s="83" t="s">
+        <v>530</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>442</v>
-      </c>
       <c r="M5" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>444</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="R5" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="T5" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>384</v>
       </c>
@@ -7266,69 +7338,73 @@
       <c r="E6" s="83">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="F6" s="83">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:28" ht="57" x14ac:dyDescent="0.45">
       <c r="D7" s="82"/>
       <c r="E7" s="84">
         <v>1</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="F7" s="84"/>
+      <c r="K7" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>500</v>
-      </c>
       <c r="L7" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="M7" s="83">
+        <v>496</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="N7" s="83">
         <v>1</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>502</v>
+      <c r="P7" s="2" t="s">
+        <v>499</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="U7" s="83">
+        <v>498</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="V7" s="83">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>373</v>
       </c>
@@ -7336,44 +7412,47 @@
         <v>397</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="E8" s="83">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="F8" s="83">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="P8" s="2" t="s">
-        <v>432</v>
+        <v>526</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>433</v>
+        <v>527</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>408</v>
+        <v>426</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
+        <v>413</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>374</v>
       </c>
@@ -7386,39 +7465,42 @@
       <c r="E9" s="83">
         <v>1</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="F9" s="83" t="s">
+        <v>531</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>438</v>
-      </c>
       <c r="P9" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:27" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:28" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>382</v>
       </c>
@@ -7426,44 +7508,47 @@
         <v>397</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E10" s="83" t="s">
         <v>400</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="F10" s="83" t="s">
+        <v>530</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J10" s="82" t="s">
-        <v>446</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="82" t="s">
+        <v>442</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="M10" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="P10" s="2" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="R10" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="S10" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="S10" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="T10" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>395</v>
       </c>
@@ -7471,44 +7556,47 @@
         <v>397</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E11" s="83">
         <v>1</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="F11" s="83" t="s">
+        <v>532</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J11" s="82" t="s">
-        <v>446</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="82" t="s">
+        <v>451</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="M11" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="P11" s="2" t="s">
-        <v>432</v>
+        <v>453</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="R11" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="S11" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="T11" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" ht="57" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>386</v>
       </c>
@@ -7521,39 +7609,42 @@
       <c r="E12" s="83">
         <v>1</v>
       </c>
-      <c r="I12" s="82" t="s">
+      <c r="F12" s="88">
+        <v>36911</v>
+      </c>
+      <c r="J12" s="82" t="s">
         <v>414</v>
       </c>
-      <c r="J12" s="82" t="s">
+      <c r="K12" s="82" t="s">
         <v>415</v>
       </c>
-      <c r="K12" s="82" t="s">
+      <c r="L12" s="82" t="s">
         <v>410</v>
       </c>
-      <c r="L12" s="82" t="s">
+      <c r="M12" s="82" t="s">
         <v>416</v>
       </c>
-      <c r="M12" s="82" t="s">
+      <c r="N12" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="O12" s="82" t="s">
+      <c r="P12" s="82" t="s">
         <v>423</v>
       </c>
-      <c r="P12" s="82" t="s">
+      <c r="Q12" s="82" t="s">
         <v>417</v>
       </c>
-      <c r="Q12" s="82" t="s">
+      <c r="R12" s="82" t="s">
         <v>411</v>
       </c>
-      <c r="R12" s="82" t="s">
+      <c r="S12" s="82" t="s">
         <v>412</v>
       </c>
-      <c r="S12" s="82" t="s">
+      <c r="T12" s="82" t="s">
         <v>418</v>
       </c>
-      <c r="U12" s="2"/>
-    </row>
-    <row r="13" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:28" ht="57" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>388</v>
       </c>
@@ -7561,44 +7652,47 @@
         <v>220</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E13" s="83">
         <v>1</v>
       </c>
-      <c r="I13" s="82" t="s">
+      <c r="F13" s="88">
+        <v>45658</v>
+      </c>
+      <c r="J13" s="82" t="s">
         <v>414</v>
       </c>
-      <c r="J13" s="82" t="s">
+      <c r="K13" s="82" t="s">
         <v>419</v>
       </c>
-      <c r="K13" s="82" t="s">
+      <c r="L13" s="82" t="s">
         <v>410</v>
       </c>
-      <c r="L13" s="82" t="s">
+      <c r="M13" s="82" t="s">
         <v>420</v>
       </c>
-      <c r="M13" s="82" t="s">
+      <c r="N13" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="O13" s="82" t="s">
+      <c r="P13" s="82" t="s">
         <v>424</v>
       </c>
-      <c r="P13" s="82" t="s">
+      <c r="Q13" s="82" t="s">
         <v>421</v>
       </c>
-      <c r="Q13" s="82" t="s">
+      <c r="R13" s="82" t="s">
         <v>411</v>
       </c>
-      <c r="R13" s="82" t="s">
+      <c r="S13" s="82" t="s">
         <v>412</v>
       </c>
-      <c r="S13" s="82" t="s">
+      <c r="T13" s="82" t="s">
         <v>422</v>
       </c>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:27" ht="57" x14ac:dyDescent="0.45">
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:28" ht="57" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>389</v>
       </c>
@@ -7611,40 +7705,43 @@
       <c r="E14" s="83">
         <v>1</v>
       </c>
-      <c r="I14" s="82" t="s">
+      <c r="F14" s="83" t="s">
+        <v>533</v>
+      </c>
+      <c r="J14" s="82" t="s">
         <v>414</v>
       </c>
-      <c r="J14" s="82" t="s">
-        <v>465</v>
-      </c>
       <c r="K14" s="82" t="s">
+        <v>461</v>
+      </c>
+      <c r="L14" s="82" t="s">
         <v>403</v>
       </c>
-      <c r="L14" s="82" t="s">
-        <v>466</v>
-      </c>
       <c r="M14" s="82" t="s">
+        <v>462</v>
+      </c>
+      <c r="N14" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82" t="s">
-        <v>522</v>
-      </c>
+      <c r="O14" s="82"/>
       <c r="P14" s="82" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="Q14" s="82" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="R14" s="82" t="s">
+        <v>519</v>
+      </c>
+      <c r="S14" s="82" t="s">
         <v>408</v>
       </c>
-      <c r="S14" s="82" t="s">
-        <v>466</v>
-      </c>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="T14" s="82" t="s">
+        <v>462</v>
+      </c>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>383</v>
       </c>
@@ -7652,44 +7749,47 @@
         <v>397</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E15" s="83" t="s">
         <v>400</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>414</v>
+      <c r="F15" s="83" t="s">
+        <v>534</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>455</v>
+        <v>401</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>456</v>
-      </c>
       <c r="M15" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>457</v>
-      </c>
       <c r="P15" s="2" t="s">
-        <v>432</v>
+        <v>522</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="R15" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="S15" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="U15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="T15" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
         <v>376</v>
       </c>
@@ -7702,78 +7802,82 @@
       <c r="E16" s="83" t="s">
         <v>399</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="F16" s="83" t="s">
+        <v>535</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>437</v>
-      </c>
       <c r="M16" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="P16" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Q16" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="S16" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="U16" s="2"/>
-    </row>
-    <row r="17" spans="2:27" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="T16" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:28" ht="71.25" x14ac:dyDescent="0.45">
       <c r="D17" s="82"/>
       <c r="E17" s="84" t="s">
-        <v>511</v>
-      </c>
-      <c r="J17" s="82" t="s">
-        <v>504</v>
-      </c>
+        <v>507</v>
+      </c>
+      <c r="F17" s="84"/>
       <c r="K17" s="82" t="s">
         <v>500</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>519</v>
-      </c>
-      <c r="M17" s="84" t="s">
-        <v>511</v>
-      </c>
-      <c r="O17" s="82" t="s">
-        <v>525</v>
+        <v>496</v>
+      </c>
+      <c r="M17" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="N17" s="84" t="s">
+        <v>507</v>
       </c>
       <c r="P17" s="82" t="s">
-        <v>443</v>
+        <v>521</v>
       </c>
       <c r="Q17" s="82" t="s">
-        <v>510</v>
+        <v>439</v>
       </c>
       <c r="R17" s="82" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="S17" s="82" t="s">
+        <v>514</v>
+      </c>
+      <c r="T17" s="82" t="s">
+        <v>503</v>
+      </c>
+      <c r="V17" s="84" t="s">
         <v>507</v>
       </c>
-      <c r="U17" s="84" t="s">
-        <v>511</v>
-      </c>
-      <c r="AA17" s="82" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="AB17" s="82" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>372</v>
       </c>
@@ -7781,44 +7885,47 @@
         <v>397</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E18" s="83">
         <v>1</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="F18" s="83" t="s">
+        <v>536</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L18" s="85" t="s">
-        <v>491</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O18" s="82" t="s">
+      <c r="P18" s="82" t="s">
         <v>405</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="Q18" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="U18" s="2"/>
-    </row>
-    <row r="19" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="2:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>392</v>
       </c>
@@ -7829,42 +7936,45 @@
       <c r="E19" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="I19" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="J19" s="2" t="s">
+      <c r="F19" s="89">
+        <v>45658</v>
+      </c>
+      <c r="J19" s="82" t="s">
+        <v>501</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="P19" s="82" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="T19" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="O19" s="82" t="s">
-        <v>469</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="U19" s="2"/>
-      <c r="AA19" s="82" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+      <c r="V19" s="2"/>
+      <c r="AB19" s="82" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" ht="114" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
         <v>393</v>
       </c>
@@ -7875,39 +7985,42 @@
       <c r="E20" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="I20" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>479</v>
+      <c r="F20" s="84" t="s">
+        <v>538</v>
+      </c>
+      <c r="J20" s="82" t="s">
+        <v>501</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="M20" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O20" s="82" t="s">
-        <v>487</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>489</v>
+      <c r="P20" s="82" t="s">
+        <v>483</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
+        <v>472</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="2:28" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
         <v>394</v>
       </c>
@@ -7918,39 +8031,42 @@
       <c r="E21" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="I21" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>480</v>
+      <c r="F21" s="89">
+        <v>45292</v>
+      </c>
+      <c r="J21" s="82" t="s">
+        <v>501</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="M21" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="O21" s="82" t="s">
-        <v>483</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>482</v>
+      <c r="P21" s="82" t="s">
+        <v>479</v>
       </c>
       <c r="Q21" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="R21" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="S21" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
+        <v>466</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="2:28" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>391</v>
       </c>
@@ -7961,39 +8077,42 @@
       <c r="E22" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="I22" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="F22" s="84" t="s">
+        <v>537</v>
+      </c>
+      <c r="J22" s="82" t="s">
+        <v>501</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="P22" s="82" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="S22" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="O22" s="82" t="s">
+      <c r="T22" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="2:28" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
         <v>396</v>
       </c>
@@ -8001,92 +8120,94 @@
         <v>357</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="F23" s="82"/>
+      <c r="F23" s="84"/>
       <c r="G23" s="82"/>
       <c r="H23" s="82"/>
-      <c r="I23" s="82" t="s">
+      <c r="I23" s="82"/>
+      <c r="J23" s="82" t="s">
         <v>401</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="K23" s="82" t="s">
+        <v>509</v>
+      </c>
+      <c r="L23" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="M23" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="N23" s="82" t="s">
+        <v>400</v>
+      </c>
+      <c r="O23" s="82"/>
+      <c r="P23" s="82" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q23" s="82" t="s">
+        <v>407</v>
+      </c>
+      <c r="R23" s="82" t="s">
+        <v>511</v>
+      </c>
+      <c r="S23" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="T23" s="82" t="s">
         <v>513</v>
       </c>
-      <c r="K23" s="82" t="s">
-        <v>512</v>
-      </c>
-      <c r="L23" s="82" t="s">
-        <v>520</v>
-      </c>
-      <c r="M23" s="82" t="s">
+      <c r="U23" s="82"/>
+      <c r="V23" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82" t="s">
-        <v>514</v>
-      </c>
-      <c r="P23" s="82" t="s">
-        <v>407</v>
-      </c>
-      <c r="Q23" s="82" t="s">
-        <v>515</v>
-      </c>
-      <c r="R23" s="82" t="s">
-        <v>516</v>
-      </c>
-      <c r="S23" s="82" t="s">
-        <v>517</v>
-      </c>
-      <c r="T23" s="82"/>
-      <c r="U23" s="82" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="2:28" ht="57" x14ac:dyDescent="0.45">
       <c r="D24" s="82"/>
       <c r="E24" s="84">
         <v>1</v>
       </c>
-      <c r="J24" s="82" t="s">
-        <v>499</v>
-      </c>
+      <c r="F24" s="84"/>
       <c r="K24" s="82" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="L24" s="82" t="s">
-        <v>506</v>
-      </c>
-      <c r="M24" s="84">
+        <v>496</v>
+      </c>
+      <c r="M24" s="82" t="s">
+        <v>502</v>
+      </c>
+      <c r="N24" s="84">
         <v>1</v>
       </c>
-      <c r="O24" s="82" t="s">
-        <v>508</v>
-      </c>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="82" t="s">
-        <v>508</v>
-      </c>
+      <c r="P24" s="82" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q24" s="82"/>
       <c r="R24" s="82" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="S24" s="82" t="s">
-        <v>506</v>
-      </c>
-      <c r="U24" s="84">
+        <v>505</v>
+      </c>
+      <c r="T24" s="82" t="s">
+        <v>502</v>
+      </c>
+      <c r="V24" s="84">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations disablePrompts="1" count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W22:W1048576 V2:V24" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="X22:X1048576 W2:W24" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>
@@ -8576,20 +8697,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Updates xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099718ADBC551F541BC88D358FCBE0BE1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="431516bc1bae45c9da16ea2d2733f767">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xmlns:ns3="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b847ca3903a29a1cc3194747c84dee6d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8843,6 +8950,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Updates xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2317584-b0e7-4f0b-a0b2-363e6e597dc0" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2666cf29-b4bf-4847-95b3-6cedd838a2fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2AE94B-495A-4017-A3D0-1724D4100D07}">
   <ds:schemaRefs>
@@ -8852,24 +8973,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B05EF41-DB28-4C2E-A8E7-8EFEC28FA29F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB52426-5EDD-49C9-B37C-4AE9ED6E055B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8887,4 +8990,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B05EF41-DB28-4C2E-A8E7-8EFEC28FA29F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2666cf29-b4bf-4847-95b3-6cedd838a2fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b2317584-b0e7-4f0b-a0b2-363e6e597dc0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>